<commit_message>
updated data fields information. highlighted in yellow is information that should be contained in metadata file
</commit_message>
<xml_diff>
--- a/raw/project_IFCB_dashboard_standardizer.xlsx
+++ b/raw/project_IFCB_dashboard_standardizer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc4214/GIT/PSSdb/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01E1F3E-DFB9-524E-9245-ED10C6EB5544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D887436-E2D0-3A45-B2C2-F012C6406C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="7380" windowWidth="27640" windowHeight="16940" xr2:uid="{82E6A812-7886-944F-84A0-B5F41EC2BEAB}"/>
+    <workbookView xWindow="1280" yWindow="3260" windowWidth="27640" windowHeight="16940" xr2:uid="{82E6A812-7886-944F-84A0-B5F41EC2BEAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="70">
   <si>
     <t>Project_ID</t>
   </si>
@@ -222,6 +222,30 @@
   </si>
   <si>
     <t>meter</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>vol_analyzed</t>
+  </si>
+  <si>
+    <t>ml</t>
+  </si>
+  <si>
+    <t>pixels</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Biovolume</t>
+  </si>
+  <si>
+    <t>cubed_pixels</t>
+  </si>
+  <si>
+    <t>columns in yellow = minimum information that should be included in metadata files</t>
   </si>
 </sst>
 </file>
@@ -268,12 +292,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -317,7 +347,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -332,15 +362,19 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -656,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{919EA166-C8DA-0547-807B-0442043911F9}">
-  <dimension ref="A1:AE24"/>
+  <dimension ref="A1:AH24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -675,10 +709,18 @@
     <col min="12" max="12" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -700,43 +742,43 @@
       <c r="G1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="7" t="s">
         <v>21</v>
       </c>
       <c r="U1" s="1" t="s">
@@ -757,10 +799,10 @@
       <c r="Z1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="7" t="s">
         <v>29</v>
       </c>
       <c r="AC1" s="1" t="s">
@@ -773,11 +815,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -798,18 +840,48 @@
       <c r="K2" t="s">
         <v>59</v>
       </c>
+      <c r="L2" t="s">
+        <v>60</v>
+      </c>
+      <c r="M2" t="s">
+        <v>61</v>
+      </c>
       <c r="N2" t="s">
         <v>60</v>
       </c>
       <c r="O2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="R2" t="s">
+        <v>63</v>
+      </c>
+      <c r="S2" t="s">
+        <v>64</v>
+      </c>
+      <c r="W2" t="s">
+        <v>67</v>
+      </c>
+      <c r="X2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH2" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -818,12 +890,57 @@
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" t="s">
+        <v>60</v>
+      </c>
+      <c r="M3" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" t="s">
+        <v>60</v>
+      </c>
+      <c r="O3" t="s">
+        <v>61</v>
+      </c>
+      <c r="R3" t="s">
+        <v>63</v>
+      </c>
+      <c r="S3" t="s">
+        <v>64</v>
+      </c>
+      <c r="W3" t="s">
+        <v>67</v>
+      </c>
+      <c r="X3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -831,12 +948,57 @@
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" t="s">
+        <v>58</v>
+      </c>
+      <c r="K4" t="s">
+        <v>59</v>
+      </c>
+      <c r="L4" t="s">
+        <v>60</v>
+      </c>
+      <c r="M4" t="s">
+        <v>61</v>
+      </c>
+      <c r="N4" t="s">
+        <v>60</v>
+      </c>
+      <c r="O4" t="s">
+        <v>61</v>
+      </c>
+      <c r="R4" t="s">
+        <v>63</v>
+      </c>
+      <c r="S4" t="s">
+        <v>64</v>
+      </c>
+      <c r="W4" t="s">
+        <v>67</v>
+      </c>
+      <c r="X4" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -844,214 +1006,1114 @@
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" t="s">
+        <v>59</v>
+      </c>
+      <c r="J5" t="s">
+        <v>58</v>
+      </c>
+      <c r="K5" t="s">
+        <v>59</v>
+      </c>
+      <c r="L5" t="s">
+        <v>60</v>
+      </c>
+      <c r="M5" t="s">
+        <v>61</v>
+      </c>
+      <c r="N5" t="s">
+        <v>60</v>
+      </c>
+      <c r="O5" t="s">
+        <v>61</v>
+      </c>
+      <c r="R5" t="s">
+        <v>63</v>
+      </c>
+      <c r="S5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W5" t="s">
+        <v>67</v>
+      </c>
+      <c r="X5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I6" t="s">
+        <v>59</v>
+      </c>
+      <c r="J6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K6" t="s">
+        <v>59</v>
+      </c>
+      <c r="L6" t="s">
+        <v>60</v>
+      </c>
+      <c r="M6" t="s">
+        <v>61</v>
+      </c>
+      <c r="N6" t="s">
+        <v>60</v>
+      </c>
+      <c r="O6" t="s">
+        <v>61</v>
+      </c>
+      <c r="R6" t="s">
+        <v>63</v>
+      </c>
+      <c r="S6" t="s">
+        <v>64</v>
+      </c>
+      <c r="W6" t="s">
+        <v>67</v>
+      </c>
+      <c r="X6" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>57</v>
+      </c>
+      <c r="I7" t="s">
+        <v>59</v>
+      </c>
+      <c r="J7" t="s">
+        <v>58</v>
+      </c>
+      <c r="K7" t="s">
+        <v>59</v>
+      </c>
+      <c r="L7" t="s">
+        <v>60</v>
+      </c>
+      <c r="M7" t="s">
+        <v>61</v>
+      </c>
+      <c r="N7" t="s">
+        <v>60</v>
+      </c>
+      <c r="O7" t="s">
+        <v>61</v>
+      </c>
+      <c r="R7" t="s">
+        <v>63</v>
+      </c>
+      <c r="S7" t="s">
+        <v>64</v>
+      </c>
+      <c r="W7" t="s">
+        <v>67</v>
+      </c>
+      <c r="X7" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" t="s">
+        <v>59</v>
+      </c>
+      <c r="J8" t="s">
+        <v>58</v>
+      </c>
+      <c r="K8" t="s">
+        <v>59</v>
+      </c>
+      <c r="L8" t="s">
+        <v>60</v>
+      </c>
+      <c r="M8" t="s">
+        <v>61</v>
+      </c>
+      <c r="N8" t="s">
+        <v>60</v>
+      </c>
+      <c r="O8" t="s">
+        <v>61</v>
+      </c>
+      <c r="R8" t="s">
+        <v>63</v>
+      </c>
+      <c r="S8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W8" t="s">
+        <v>67</v>
+      </c>
+      <c r="X8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" t="s">
+        <v>59</v>
+      </c>
+      <c r="J9" t="s">
+        <v>58</v>
+      </c>
+      <c r="K9" t="s">
+        <v>59</v>
+      </c>
+      <c r="L9" t="s">
+        <v>60</v>
+      </c>
+      <c r="M9" t="s">
+        <v>61</v>
+      </c>
+      <c r="N9" t="s">
+        <v>60</v>
+      </c>
+      <c r="O9" t="s">
+        <v>61</v>
+      </c>
+      <c r="R9" t="s">
+        <v>63</v>
+      </c>
+      <c r="S9" t="s">
+        <v>64</v>
+      </c>
+      <c r="W9" t="s">
+        <v>67</v>
+      </c>
+      <c r="X9" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I10" t="s">
+        <v>59</v>
+      </c>
+      <c r="J10" t="s">
+        <v>58</v>
+      </c>
+      <c r="K10" t="s">
+        <v>59</v>
+      </c>
+      <c r="L10" t="s">
+        <v>60</v>
+      </c>
+      <c r="M10" t="s">
+        <v>61</v>
+      </c>
+      <c r="N10" t="s">
+        <v>60</v>
+      </c>
+      <c r="O10" t="s">
+        <v>61</v>
+      </c>
+      <c r="R10" t="s">
+        <v>63</v>
+      </c>
+      <c r="S10" t="s">
+        <v>64</v>
+      </c>
+      <c r="W10" t="s">
+        <v>67</v>
+      </c>
+      <c r="X10" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="H11" t="s">
+        <v>57</v>
+      </c>
+      <c r="I11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J11" t="s">
+        <v>58</v>
+      </c>
+      <c r="K11" t="s">
+        <v>59</v>
+      </c>
+      <c r="L11" t="s">
+        <v>60</v>
+      </c>
+      <c r="M11" t="s">
+        <v>61</v>
+      </c>
+      <c r="N11" t="s">
+        <v>60</v>
+      </c>
+      <c r="O11" t="s">
+        <v>61</v>
+      </c>
+      <c r="R11" t="s">
+        <v>63</v>
+      </c>
+      <c r="S11" t="s">
+        <v>64</v>
+      </c>
+      <c r="W11" t="s">
+        <v>67</v>
+      </c>
+      <c r="X11" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="H12" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" t="s">
+        <v>59</v>
+      </c>
+      <c r="J12" t="s">
+        <v>58</v>
+      </c>
+      <c r="K12" t="s">
+        <v>59</v>
+      </c>
+      <c r="L12" t="s">
+        <v>60</v>
+      </c>
+      <c r="M12" t="s">
+        <v>61</v>
+      </c>
+      <c r="N12" t="s">
+        <v>60</v>
+      </c>
+      <c r="O12" t="s">
+        <v>61</v>
+      </c>
+      <c r="R12" t="s">
+        <v>63</v>
+      </c>
+      <c r="S12" t="s">
+        <v>64</v>
+      </c>
+      <c r="W12" t="s">
+        <v>67</v>
+      </c>
+      <c r="X12" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="H13" t="s">
+        <v>57</v>
+      </c>
+      <c r="I13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J13" t="s">
+        <v>58</v>
+      </c>
+      <c r="K13" t="s">
+        <v>59</v>
+      </c>
+      <c r="L13" t="s">
+        <v>60</v>
+      </c>
+      <c r="M13" t="s">
+        <v>61</v>
+      </c>
+      <c r="N13" t="s">
+        <v>60</v>
+      </c>
+      <c r="O13" t="s">
+        <v>61</v>
+      </c>
+      <c r="R13" t="s">
+        <v>63</v>
+      </c>
+      <c r="S13" t="s">
+        <v>64</v>
+      </c>
+      <c r="W13" t="s">
+        <v>67</v>
+      </c>
+      <c r="X13" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>57</v>
+      </c>
+      <c r="I14" t="s">
+        <v>59</v>
+      </c>
+      <c r="J14" t="s">
+        <v>58</v>
+      </c>
+      <c r="K14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L14" t="s">
+        <v>60</v>
+      </c>
+      <c r="M14" t="s">
+        <v>61</v>
+      </c>
+      <c r="N14" t="s">
+        <v>60</v>
+      </c>
+      <c r="O14" t="s">
+        <v>61</v>
+      </c>
+      <c r="R14" t="s">
+        <v>63</v>
+      </c>
+      <c r="S14" t="s">
+        <v>64</v>
+      </c>
+      <c r="W14" t="s">
+        <v>67</v>
+      </c>
+      <c r="X14" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>57</v>
+      </c>
+      <c r="I15" t="s">
+        <v>59</v>
+      </c>
+      <c r="J15" t="s">
+        <v>58</v>
+      </c>
+      <c r="K15" t="s">
+        <v>59</v>
+      </c>
+      <c r="L15" t="s">
+        <v>60</v>
+      </c>
+      <c r="M15" t="s">
+        <v>61</v>
+      </c>
+      <c r="N15" t="s">
+        <v>60</v>
+      </c>
+      <c r="O15" t="s">
+        <v>61</v>
+      </c>
+      <c r="R15" t="s">
+        <v>63</v>
+      </c>
+      <c r="S15" t="s">
+        <v>64</v>
+      </c>
+      <c r="W15" t="s">
+        <v>67</v>
+      </c>
+      <c r="X15" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C16" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H16" t="s">
+        <v>57</v>
+      </c>
+      <c r="I16" t="s">
+        <v>59</v>
+      </c>
+      <c r="J16" t="s">
+        <v>58</v>
+      </c>
+      <c r="K16" t="s">
+        <v>59</v>
+      </c>
+      <c r="L16" t="s">
+        <v>60</v>
+      </c>
+      <c r="M16" t="s">
+        <v>61</v>
+      </c>
+      <c r="N16" t="s">
+        <v>60</v>
+      </c>
+      <c r="O16" t="s">
+        <v>61</v>
+      </c>
+      <c r="R16" t="s">
+        <v>63</v>
+      </c>
+      <c r="S16" t="s">
+        <v>64</v>
+      </c>
+      <c r="W16" t="s">
+        <v>67</v>
+      </c>
+      <c r="X16" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C17" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H17" t="s">
+        <v>57</v>
+      </c>
+      <c r="I17" t="s">
+        <v>59</v>
+      </c>
+      <c r="J17" t="s">
+        <v>58</v>
+      </c>
+      <c r="K17" t="s">
+        <v>59</v>
+      </c>
+      <c r="L17" t="s">
+        <v>60</v>
+      </c>
+      <c r="M17" t="s">
+        <v>61</v>
+      </c>
+      <c r="N17" t="s">
+        <v>60</v>
+      </c>
+      <c r="O17" t="s">
+        <v>61</v>
+      </c>
+      <c r="R17" t="s">
+        <v>63</v>
+      </c>
+      <c r="S17" t="s">
+        <v>64</v>
+      </c>
+      <c r="W17" t="s">
+        <v>67</v>
+      </c>
+      <c r="X17" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C18" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H18" t="s">
+        <v>57</v>
+      </c>
+      <c r="I18" t="s">
+        <v>59</v>
+      </c>
+      <c r="J18" t="s">
+        <v>58</v>
+      </c>
+      <c r="K18" t="s">
+        <v>59</v>
+      </c>
+      <c r="L18" t="s">
+        <v>60</v>
+      </c>
+      <c r="M18" t="s">
+        <v>61</v>
+      </c>
+      <c r="N18" t="s">
+        <v>60</v>
+      </c>
+      <c r="O18" t="s">
+        <v>61</v>
+      </c>
+      <c r="R18" t="s">
+        <v>63</v>
+      </c>
+      <c r="S18" t="s">
+        <v>64</v>
+      </c>
+      <c r="W18" t="s">
+        <v>67</v>
+      </c>
+      <c r="X18" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C19" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H19" t="s">
+        <v>57</v>
+      </c>
+      <c r="I19" t="s">
+        <v>59</v>
+      </c>
+      <c r="J19" t="s">
+        <v>58</v>
+      </c>
+      <c r="K19" t="s">
+        <v>59</v>
+      </c>
+      <c r="L19" t="s">
+        <v>60</v>
+      </c>
+      <c r="M19" t="s">
+        <v>61</v>
+      </c>
+      <c r="N19" t="s">
+        <v>60</v>
+      </c>
+      <c r="O19" t="s">
+        <v>61</v>
+      </c>
+      <c r="R19" t="s">
+        <v>63</v>
+      </c>
+      <c r="S19" t="s">
+        <v>64</v>
+      </c>
+      <c r="W19" t="s">
+        <v>67</v>
+      </c>
+      <c r="X19" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C20" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H20" t="s">
+        <v>57</v>
+      </c>
+      <c r="I20" t="s">
+        <v>59</v>
+      </c>
+      <c r="J20" t="s">
+        <v>58</v>
+      </c>
+      <c r="K20" t="s">
+        <v>59</v>
+      </c>
+      <c r="L20" t="s">
+        <v>60</v>
+      </c>
+      <c r="M20" t="s">
+        <v>61</v>
+      </c>
+      <c r="N20" t="s">
+        <v>60</v>
+      </c>
+      <c r="O20" t="s">
+        <v>61</v>
+      </c>
+      <c r="R20" t="s">
+        <v>63</v>
+      </c>
+      <c r="S20" t="s">
+        <v>64</v>
+      </c>
+      <c r="W20" t="s">
+        <v>67</v>
+      </c>
+      <c r="X20" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C21" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H21" t="s">
+        <v>57</v>
+      </c>
+      <c r="I21" t="s">
+        <v>59</v>
+      </c>
+      <c r="J21" t="s">
+        <v>58</v>
+      </c>
+      <c r="K21" t="s">
+        <v>59</v>
+      </c>
+      <c r="L21" t="s">
+        <v>60</v>
+      </c>
+      <c r="M21" t="s">
+        <v>61</v>
+      </c>
+      <c r="N21" t="s">
+        <v>60</v>
+      </c>
+      <c r="O21" t="s">
+        <v>61</v>
+      </c>
+      <c r="R21" t="s">
+        <v>63</v>
+      </c>
+      <c r="S21" t="s">
+        <v>64</v>
+      </c>
+      <c r="W21" t="s">
+        <v>67</v>
+      </c>
+      <c r="X21" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C22" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H22" t="s">
+        <v>57</v>
+      </c>
+      <c r="I22" t="s">
+        <v>59</v>
+      </c>
+      <c r="J22" t="s">
+        <v>58</v>
+      </c>
+      <c r="K22" t="s">
+        <v>59</v>
+      </c>
+      <c r="L22" t="s">
+        <v>60</v>
+      </c>
+      <c r="M22" t="s">
+        <v>61</v>
+      </c>
+      <c r="N22" t="s">
+        <v>60</v>
+      </c>
+      <c r="O22" t="s">
+        <v>61</v>
+      </c>
+      <c r="R22" t="s">
+        <v>63</v>
+      </c>
+      <c r="S22" t="s">
+        <v>64</v>
+      </c>
+      <c r="W22" t="s">
+        <v>67</v>
+      </c>
+      <c r="X22" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C23" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H23" t="s">
+        <v>57</v>
+      </c>
+      <c r="I23" t="s">
+        <v>59</v>
+      </c>
+      <c r="J23" t="s">
+        <v>58</v>
+      </c>
+      <c r="K23" t="s">
+        <v>59</v>
+      </c>
+      <c r="L23" t="s">
+        <v>60</v>
+      </c>
+      <c r="M23" t="s">
+        <v>61</v>
+      </c>
+      <c r="N23" t="s">
+        <v>60</v>
+      </c>
+      <c r="O23" t="s">
+        <v>61</v>
+      </c>
+      <c r="R23" t="s">
+        <v>63</v>
+      </c>
+      <c r="S23" t="s">
+        <v>64</v>
+      </c>
+      <c r="W23" t="s">
+        <v>67</v>
+      </c>
+      <c r="X23" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C24" t="s">
         <v>47</v>
+      </c>
+      <c r="H24" t="s">
+        <v>57</v>
+      </c>
+      <c r="I24" t="s">
+        <v>59</v>
+      </c>
+      <c r="J24" t="s">
+        <v>58</v>
+      </c>
+      <c r="K24" t="s">
+        <v>59</v>
+      </c>
+      <c r="L24" t="s">
+        <v>60</v>
+      </c>
+      <c r="M24" t="s">
+        <v>61</v>
+      </c>
+      <c r="N24" t="s">
+        <v>60</v>
+      </c>
+      <c r="O24" t="s">
+        <v>61</v>
+      </c>
+      <c r="R24" t="s">
+        <v>63</v>
+      </c>
+      <c r="S24" t="s">
+        <v>64</v>
+      </c>
+      <c r="W24" t="s">
+        <v>67</v>
+      </c>
+      <c r="X24" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>